<commit_message>
Updates to json format as updates have been done to the filewriter
</commit_message>
<xml_diff>
--- a/examples/odin/config.xlsx
+++ b/examples/odin/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenanmuric/Code/DMSC/generate-nexus-files/examples/odin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C1879C-FE8B-8142-9F83-5C9912909CA0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0F38F7-CCAF-2142-98B0-D30EB048CAD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14280" yWindow="9760" windowWidth="28040" windowHeight="17440" xr2:uid="{8DB84DE1-9EED-394B-A2C5-2E8B6120B41D}"/>
+    <workbookView xWindow="6620" yWindow="9780" windowWidth="36560" windowHeight="17440" xr2:uid="{8DB84DE1-9EED-394B-A2C5-2E8B6120B41D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
-  <si>
-    <t>writer_module</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>source</t>
   </si>
@@ -85,16 +82,38 @@
   </si>
   <si>
     <t>topic</t>
+  </si>
+  <si>
+    <t>dtype</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>value_units</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>module</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -120,9 +139,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -441,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD0A6C8-CD12-C54F-919F-A5E3FEC98221}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="234" zoomScaleNormal="234" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -456,81 +478,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
+      <c r="G1" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>

</xml_diff>

<commit_message>
light tomography filewriting work
</commit_message>
<xml_diff>
--- a/examples/odin/config.xlsx
+++ b/examples/odin/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenanmuric/Code/DMSC/generate-nexus-files/examples/odin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0F38F7-CCAF-2142-98B0-D30EB048CAD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6F80DA-3A74-8246-BB53-73EE9E0716F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6620" yWindow="9780" windowWidth="36560" windowHeight="17440" xr2:uid="{8DB84DE1-9EED-394B-A2C5-2E8B6120B41D}"/>
+    <workbookView xWindow="10480" yWindow="9000" windowWidth="36560" windowHeight="17440" xr2:uid="{8DB84DE1-9EED-394B-A2C5-2E8B6120B41D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,56 +25,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>source</t>
   </si>
   <si>
-    <t>Nxdetector</t>
-  </si>
-  <si>
     <t>detector</t>
   </si>
   <si>
-    <t>Nxsamle</t>
-  </si>
-  <si>
     <t>sample</t>
   </si>
   <si>
-    <t>NXMonitor</t>
-  </si>
-  <si>
     <t>control</t>
   </si>
   <si>
-    <t>Nxdata</t>
-  </si>
-  <si>
     <t>data</t>
   </si>
   <si>
-    <t>Topic_1</t>
-  </si>
-  <si>
-    <t>Topic_2</t>
-  </si>
-  <si>
-    <t>Topic_3</t>
-  </si>
-  <si>
-    <t>f142</t>
-  </si>
-  <si>
-    <t>d1</t>
-  </si>
-  <si>
-    <t>PV:my_pv2</t>
-  </si>
-  <si>
-    <t>mon1</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -87,16 +54,40 @@
     <t>dtype</t>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
     <t>value_units</t>
   </si>
   <si>
-    <t>mm</t>
-  </si>
-  <si>
     <t>module</t>
+  </si>
+  <si>
+    <t>odin_topic</t>
+  </si>
+  <si>
+    <t>NXdata</t>
+  </si>
+  <si>
+    <t>NXdetector</t>
+  </si>
+  <si>
+    <t>NXmonitor</t>
+  </si>
+  <si>
+    <t>image_source</t>
+  </si>
+  <si>
+    <t>ADAr</t>
+  </si>
+  <si>
+    <t>NXsample</t>
+  </si>
+  <si>
+    <t>uint32</t>
+  </si>
+  <si>
+    <t>array_size</t>
+  </si>
+  <si>
+    <t>480, 290, 3</t>
   </si>
 </sst>
 </file>
@@ -461,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD0A6C8-CD12-C54F-919F-A5E3FEC98221}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="234" zoomScaleNormal="234" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="234" zoomScaleNormal="234" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -477,112 +468,96 @@
     <col min="7" max="7" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -591,7 +566,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -600,7 +575,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -609,21 +584,21 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>

</xml_diff>

<commit_message>
adding additional data sets for dark current and open beam images
</commit_message>
<xml_diff>
--- a/examples/odin/config.xlsx
+++ b/examples/odin/config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenanmuric/Code/DMSC/generate-nexus-files/examples/odin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenanmuric/Code/DMSC/light-tomography-nexus/examples/odin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6F80DA-3A74-8246-BB53-73EE9E0716F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D16296A-9A23-854A-990C-19A5F0A7DD75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10480" yWindow="9000" windowWidth="36560" windowHeight="17440" xr2:uid="{8DB84DE1-9EED-394B-A2C5-2E8B6120B41D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>source</t>
   </si>
@@ -88,13 +88,34 @@
   </si>
   <si>
     <t>480, 290, 3</t>
+  </si>
+  <si>
+    <t>data_dark</t>
+  </si>
+  <si>
+    <t>data_flat</t>
+  </si>
+  <si>
+    <t>image_dark</t>
+  </si>
+  <si>
+    <t>image_flat</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>custom_field</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -108,6 +129,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
   <fills count="2">
@@ -130,12 +156,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -452,23 +481,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD0A6C8-CD12-C54F-919F-A5E3FEC98221}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="234" zoomScaleNormal="234" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="234" zoomScaleNormal="234" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" customWidth="1"/>
-    <col min="7" max="7" width="29.5" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -493,8 +523,11 @@
       <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -506,8 +539,11 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -519,8 +555,11 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -532,8 +571,11 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -556,26 +598,65 @@
       <c r="H5" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -584,21 +665,21 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>

</xml_diff>

<commit_message>
refactoring code to better comply with the NXtomo template
</commit_message>
<xml_diff>
--- a/examples/odin/config.xlsx
+++ b/examples/odin/config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenanmuric/Code/DMSC/light-tomography-nexus/examples/odin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenanmuric/Code/DMSC/generate-nexus-files/examples/odin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D16296A-9A23-854A-990C-19A5F0A7DD75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0B13C7-CFE1-F248-8E3E-6A5ED300E499}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10480" yWindow="9000" windowWidth="36560" windowHeight="17440" xr2:uid="{8DB84DE1-9EED-394B-A2C5-2E8B6120B41D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>source</t>
   </si>
@@ -90,25 +90,25 @@
     <t>480, 290, 3</t>
   </si>
   <si>
-    <t>data_dark</t>
-  </si>
-  <si>
-    <t>data_flat</t>
-  </si>
-  <si>
-    <t>image_dark</t>
-  </si>
-  <si>
-    <t>image_flat</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
     <t>custom_field</t>
+  </si>
+  <si>
+    <t>image_key</t>
+  </si>
+  <si>
+    <t>rotation_angle</t>
+  </si>
+  <si>
+    <t>f142</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>data_name</t>
   </si>
 </sst>
 </file>
@@ -481,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD0A6C8-CD12-C54F-919F-A5E3FEC98221}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="234" zoomScaleNormal="234" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -493,12 +493,13 @@
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -526,61 +527,76 @@
       <c r="I1" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>24</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="I3" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="I4" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="H4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
@@ -599,15 +615,18 @@
         <v>20</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>4</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
@@ -616,47 +635,29 @@
         <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="I6" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -664,22 +665,23 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>

</xml_diff>

<commit_message>
added source and other fields necessary in the nxtomo application class
</commit_message>
<xml_diff>
--- a/examples/odin/config.xlsx
+++ b/examples/odin/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenanmuric/Code/DMSC/generate-nexus-files/examples/odin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0B13C7-CFE1-F248-8E3E-6A5ED300E499}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9A40F0-6A75-2148-B328-44BAC5543B9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10480" yWindow="9000" windowWidth="36560" windowHeight="17440" xr2:uid="{8DB84DE1-9EED-394B-A2C5-2E8B6120B41D}"/>
+    <workbookView xWindow="9920" yWindow="9900" windowWidth="36560" windowHeight="17440" xr2:uid="{8DB84DE1-9EED-394B-A2C5-2E8B6120B41D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
   <si>
     <t>source</t>
   </si>
@@ -90,9 +90,6 @@
     <t>480, 290, 3</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>custom_field</t>
   </si>
   <si>
@@ -109,6 +106,45 @@
   </si>
   <si>
     <t>data_name</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>probe</t>
+  </si>
+  <si>
+    <t>NXsource</t>
+  </si>
+  <si>
+    <t>static_value</t>
+  </si>
+  <si>
+    <t>x-ray</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>kind</t>
+  </si>
+  <si>
+    <t>static_data</t>
+  </si>
+  <si>
+    <t>entry</t>
+  </si>
+  <si>
+    <t>definition</t>
+  </si>
+  <si>
+    <t>NXtomo</t>
+  </si>
+  <si>
+    <t>NXentry</t>
+  </si>
+  <si>
+    <t>lego</t>
   </si>
 </sst>
 </file>
@@ -481,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD0A6C8-CD12-C54F-919F-A5E3FEC98221}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="234" zoomScaleNormal="234" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -499,7 +535,7 @@
     <col min="10" max="10" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -525,13 +561,19 @@
         <v>19</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>30</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -542,39 +584,50 @@
         <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="G2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>23</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="G3" s="1"/>
-      <c r="J3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="I3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -587,11 +640,12 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="J4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -617,11 +671,12 @@
       <c r="I5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5" s="1"/>
+      <c r="L5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -632,56 +687,105 @@
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="I8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="I9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:12">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -690,5 +794,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixing source probe and image_key data type
</commit_message>
<xml_diff>
--- a/examples/odin/config.xlsx
+++ b/examples/odin/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenanmuric/Code/DMSC/generate-nexus-files/examples/odin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9A40F0-6A75-2148-B328-44BAC5543B9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410F2BE3-7047-5443-BB64-CA27FA5C8B4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9920" yWindow="9900" windowWidth="36560" windowHeight="17440" xr2:uid="{8DB84DE1-9EED-394B-A2C5-2E8B6120B41D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
     <t>source</t>
   </si>
@@ -120,9 +120,6 @@
     <t>static_value</t>
   </si>
   <si>
-    <t>x-ray</t>
-  </si>
-  <si>
     <t>group</t>
   </si>
   <si>
@@ -145,6 +142,12 @@
   </si>
   <si>
     <t>lego</t>
+  </si>
+  <si>
+    <t>visible light</t>
+  </si>
+  <si>
+    <t>int</t>
   </si>
 </sst>
 </file>
@@ -520,7 +523,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="234" zoomScaleNormal="234" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -570,7 +573,7 @@
         <v>21</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -598,7 +601,7 @@
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -616,7 +619,7 @@
         <v>24</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="G3" s="1"/>
       <c r="I3" s="1" t="s">
@@ -624,7 +627,7 @@
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -642,7 +645,7 @@
       <c r="H4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -673,7 +676,7 @@
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -693,7 +696,7 @@
         <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="G6" s="1"/>
       <c r="I6" s="1" t="s">
@@ -701,7 +704,7 @@
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -722,19 +725,19 @@
         <v>28</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -745,13 +748,13 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="L8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -772,10 +775,10 @@
         <v>6</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:12">

</xml_diff>

<commit_message>
updated config file for light tomo
</commit_message>
<xml_diff>
--- a/examples/odin/config.xlsx
+++ b/examples/odin/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenanmuric/Code/DMSC/generate-nexus-files/examples/odin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410F2BE3-7047-5443-BB64-CA27FA5C8B4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9987F7CC-7769-364F-84DA-CB3C588A11E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9920" yWindow="9900" windowWidth="36560" windowHeight="17440" xr2:uid="{8DB84DE1-9EED-394B-A2C5-2E8B6120B41D}"/>
+    <workbookView xWindow="0" yWindow="3980" windowWidth="35840" windowHeight="17440" xr2:uid="{8DB84DE1-9EED-394B-A2C5-2E8B6120B41D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
   <si>
     <t>source</t>
   </si>
@@ -60,9 +60,6 @@
     <t>module</t>
   </si>
   <si>
-    <t>odin_topic</t>
-  </si>
-  <si>
     <t>NXdata</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>NXmonitor</t>
   </si>
   <si>
-    <t>image_source</t>
-  </si>
-  <si>
     <t>ADAr</t>
   </si>
   <si>
@@ -87,9 +81,6 @@
     <t>array_size</t>
   </si>
   <si>
-    <t>480, 290, 3</t>
-  </si>
-  <si>
     <t>custom_field</t>
   </si>
   <si>
@@ -148,6 +139,24 @@
   </si>
   <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>ymir_camera</t>
+  </si>
+  <si>
+    <t>some_source</t>
+  </si>
+  <si>
+    <t>other_source</t>
+  </si>
+  <si>
+    <t>ymir_motion</t>
+  </si>
+  <si>
+    <t>650, 650</t>
+  </si>
+  <si>
+    <t>SES-SCAN:MC-MCU-001:m4.RBV</t>
   </si>
 </sst>
 </file>
@@ -523,14 +532,14 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="234" zoomScaleNormal="234" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
     <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
@@ -561,65 +570,67 @@
         <v>9</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1"/>
       <c r="I3" s="1" t="s">
@@ -627,12 +638,12 @@
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -645,71 +656,71 @@
       <c r="H4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>0</v>
@@ -718,48 +729,48 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>2</v>
@@ -768,17 +779,17 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G9" s="1"/>
       <c r="I9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:12">

</xml_diff>